<commit_message>
To change BTL's bug（You can get results directly from the exit）. To change record share method. To change some layouts and icons.
</commit_message>
<xml_diff>
--- a/Standard/Software/The Comparison table of Software English Abbreviation.xlsx
+++ b/Standard/Software/The Comparison table of Software English Abbreviation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Full name</t>
   </si>
@@ -112,6 +112,22 @@
   </si>
   <si>
     <t>Department</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Absolutely Wrong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AW.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -283,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -310,6 +326,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -691,10 +710,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -745,8 +764,8 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
     </row>
     <row r="7" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
@@ -765,8 +784,8 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
     </row>
     <row r="10" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
@@ -778,53 +797,69 @@
     </row>
     <row r="11" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>20</v>
+        <v>31</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
+      <c r="A15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="1:2" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
+    <row r="19" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -832,7 +867,7 @@
   <mergeCells count="3">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>